<commit_message>
Modify surprised excel file
</commit_message>
<xml_diff>
--- a/dataset/surprised.xlsx
+++ b/dataset/surprised.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\이세미\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\semi\AdvancedML_project\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA1F456-8354-4B87-BE05-5D16C1DF8B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3742CA-91D0-434D-A5A6-F1DE2C9687F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8934" uniqueCount="4468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8772" uniqueCount="4387">
   <si>
     <t>1</t>
   </si>
@@ -70,9 +70,6 @@
     <t>며칠전 꿈이 너무 충격적이고 생생하여</t>
   </si>
   <si>
-    <t>싸이월드 깜짝링크 걸기</t>
-  </si>
-  <si>
     <t xml:space="preserve">'놀라운,경악할만한' 의 뜻을가진... </t>
   </si>
   <si>
@@ -112,12 +109,6 @@
     <t>갑작스러운 발기력 저하</t>
   </si>
   <si>
-    <t>기절을 영어로 어떻게 쓰나요??</t>
-  </si>
-  <si>
-    <t>기막힌외출3 방송시간, 채널</t>
-  </si>
-  <si>
     <t>수면중 움찔 거리는 증상, 왜 그런거죠?</t>
   </si>
   <si>
@@ -181,9 +172,6 @@
     <t>저혈압 어지러움 기절 발열</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출 시즌6 네버다이 10화 2012 06... </t>
-  </si>
-  <si>
     <t>자꾸 뇌에서 깜짝깜짝 놀라는느낌이 나고..</t>
   </si>
   <si>
@@ -247,9 +235,6 @@
     <t>갑작스러운 소화불량과 변비 증상</t>
   </si>
   <si>
-    <t>기막힌외출 유상무 신발 어디껀가요?</t>
-  </si>
-  <si>
     <t>화나면 기절하는 현상</t>
   </si>
   <si>
@@ -592,9 +577,6 @@
     <t xml:space="preserve">어버이날문자 어버이날문자 기막힌것좀... </t>
   </si>
   <si>
-    <t>기막힌외출에서 나온 노래</t>
-  </si>
-  <si>
     <t xml:space="preserve">기이한 모양(기뢰)의 식물 입니다. 궁금... </t>
   </si>
   <si>
@@ -856,9 +838,6 @@
     <t>가레스 베리, 케빈 놀란 선수들...</t>
   </si>
   <si>
-    <t>반면 아직은 활동중인 기막힌외출 시즌 3</t>
-  </si>
-  <si>
     <t>기절놀이하다가</t>
   </si>
   <si>
@@ -955,9 +934,6 @@
     <t>도적..기절시키기..</t>
   </si>
   <si>
-    <t>기막힌외출 몇번이예요??</t>
-  </si>
-  <si>
     <t>수면놀라움 움찔움찔놀래요</t>
   </si>
   <si>
@@ -982,9 +958,6 @@
     <t xml:space="preserve">오늘은 충격적인 날입니다. 파문된... </t>
   </si>
   <si>
-    <t>영어로 근육이 놀란걸 뭐라말하죠 아님</t>
-  </si>
-  <si>
     <t>햄스터기절</t>
   </si>
   <si>
@@ -1069,9 +1042,6 @@
     <t>볼튼의 케빈놀란에 대해 알려주세요</t>
   </si>
   <si>
-    <t>영어로 3줄 급작....굽신</t>
-  </si>
-  <si>
     <t>여자친구 깜짝이벤트</t>
   </si>
   <si>
@@ -1207,9 +1177,6 @@
     <t>기절놀이에 대해서...;;;</t>
   </si>
   <si>
-    <t>기막힌외출 리턴드 8회 때 나오던 노래</t>
-  </si>
-  <si>
     <t>놀란걸까요?</t>
   </si>
   <si>
@@ -1453,18 +1420,12 @@
     <t>비닐봉투로 기절하기 ㅠ 봐주세요 제발</t>
   </si>
   <si>
-    <t xml:space="preserve">티켓링크에서 하는 깜짝 티켓에 관한... </t>
-  </si>
-  <si>
     <t>의사쌤이 배를 누르는데 움찔 했어요-_-</t>
   </si>
   <si>
     <t xml:space="preserve">svchost.exe가 경이로운 메모리 수치를... </t>
   </si>
   <si>
-    <t>'기절하듯이 잤다'를 영어로</t>
-  </si>
-  <si>
     <t>아이쿠 색이시커매지고있습니다.</t>
   </si>
   <si>
@@ -1513,9 +1474,6 @@
     <t>도둑을 기절시키면? 죽이면 ?</t>
   </si>
   <si>
-    <t>기막힌외출 시즌1에서 나오는 곡이름(링크)</t>
-  </si>
-  <si>
     <t xml:space="preserve">일렉기타 확실하고 기막힌 연습법... </t>
   </si>
   <si>
@@ -2026,9 +1984,6 @@
     <t>기절 발작.. 제 병명이 뭔지 모르겠습니다.</t>
   </si>
   <si>
-    <t>기막힌외출 잇잖아여</t>
-  </si>
-  <si>
     <t>기절에 대한 질문이요</t>
   </si>
   <si>
@@ -2197,9 +2152,6 @@
     <t>기절</t>
   </si>
   <si>
-    <t>기막힌외출배경</t>
-  </si>
-  <si>
     <t>깜짝 아침밥을...</t>
   </si>
   <si>
@@ -2278,9 +2230,6 @@
     <t>칼에배이고 기절</t>
   </si>
   <si>
-    <t>기막힌외출시즌3</t>
-  </si>
-  <si>
     <t>라식수술 중에 기절하면</t>
   </si>
   <si>
@@ -2314,9 +2263,6 @@
     <t>전화를 오래 했더니 기절할거같아요.</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출2 미녀6인방 편에서 김준호가... </t>
-  </si>
-  <si>
     <t xml:space="preserve">주인의 횡포로 전세를 빼야하는 기막힌... </t>
   </si>
   <si>
@@ -2473,9 +2419,6 @@
     <t xml:space="preserve">제가 이번에 검진을 했는데 깜짝 놀라게... </t>
   </si>
   <si>
-    <t>기막힌외출다시보기</t>
-  </si>
-  <si>
     <t>자려다가 움찔거리면서 계속 깨요..</t>
   </si>
   <si>
@@ -2587,9 +2530,6 @@
     <t xml:space="preserve">하늘이 무섭지도 않은가 봅니다 경악... </t>
   </si>
   <si>
-    <t>기막힌외출 시즌3 왜 유상무는안나오나요?</t>
-  </si>
-  <si>
     <t>방금 기절하다가 깨어났어요</t>
   </si>
   <si>
@@ -2635,9 +2575,6 @@
     <t>제가 친구랑 기절놀이를 하는데요/;</t>
   </si>
   <si>
-    <t>기막힌외출의 개식스에서요</t>
-  </si>
-  <si>
     <t>어지러웠다가 잠시 기절했어요..</t>
   </si>
   <si>
@@ -2647,9 +2584,6 @@
     <t>제가 군인인데 술먹다 취해서 기절해서</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출에서 이부분 배경음악... </t>
-  </si>
-  <si>
     <t>눈 깜짝할사이 서른셋 명보라는 누구인</t>
   </si>
   <si>
@@ -3277,9 +3211,6 @@
     <t>기절뇌손상</t>
   </si>
   <si>
-    <t>기막힌외출 갑을전쟁에서 오프닝음악</t>
-  </si>
-  <si>
     <t>생리를 안하는데 갑작스러운 음주와 흡</t>
   </si>
   <si>
@@ -3604,9 +3535,6 @@
     <t>귀먹은 중 마 캐듯 눈도 깜짝 안한다.</t>
   </si>
   <si>
-    <t>기막힌외출 1,2,3,4 다볼수있는곳.</t>
-  </si>
-  <si>
     <t xml:space="preserve">살면서 가장 기이한 체험이라든가... </t>
   </si>
   <si>
@@ -3676,9 +3604,6 @@
     <t>저기 동영상,사진 그 움찔가튼거</t>
   </si>
   <si>
-    <t>기막힌 밤이었어. 영어로</t>
-  </si>
-  <si>
     <t xml:space="preserve">황당하고 기막힌 능력, 독특한 능력... </t>
   </si>
   <si>
@@ -4114,9 +4039,6 @@
     <t>이 사진보고 놀란게 유아도 얼굴 작은</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출 리턴즈 써리원게임 유상무가... </t>
-  </si>
-  <si>
     <t>오늘 기절햇는데요ㅠㅠㅠ</t>
   </si>
   <si>
@@ -4603,9 +4525,6 @@
     <t>기막힌 실제상황</t>
   </si>
   <si>
-    <t xml:space="preserve">블로그에 초특가할인, 깜짝특가 등 링크... </t>
-  </si>
-  <si>
     <t>깜짝놀라면 귀가 빨개지나요?</t>
   </si>
   <si>
@@ -4672,9 +4591,6 @@
     <t>누워있다가 기절</t>
   </si>
   <si>
-    <t>기막힌외출2-더웃긴밤3</t>
-  </si>
-  <si>
     <t>우주에서 일어나는 기이한 현상들</t>
   </si>
   <si>
@@ -4786,9 +4702,6 @@
     <t>깜짝놀라서 아직도 심장이 뛰어요</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출리턴즈3회... </t>
-  </si>
-  <si>
     <t>꿈해몽좀 부탁드려요 너무 충격적입니다</t>
   </si>
   <si>
@@ -4960,9 +4873,6 @@
     <t>격투기 스파링 중 기절</t>
   </si>
   <si>
-    <t>기막힌외출 시즌3</t>
-  </si>
-  <si>
     <t>미달이 김성은 충격적인 셀카영상 있나요.?</t>
   </si>
   <si>
@@ -5086,9 +4996,6 @@
     <t>죽은 엘렌은 당황스러운 표정이었다.</t>
   </si>
   <si>
-    <t>기막힌외출 배경음악 질문합니다.</t>
-  </si>
-  <si>
     <t>채팅방 방장이 예전 남친이라 놀란꿈.</t>
   </si>
   <si>
@@ -5176,9 +5083,6 @@
     <t>카톡할때 놀란대답이나 그냥대답 하는</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출 리턴즈 마지막회... </t>
-  </si>
-  <si>
     <t xml:space="preserve">이휘재 상플에서 깜짝고백... </t>
   </si>
   <si>
@@ -5323,9 +5227,6 @@
     <t xml:space="preserve">크게 깜짝 놀랐을 때 온몸에 전기오는... </t>
   </si>
   <si>
-    <t>깜짝놀랄만한상황을 사자성어로 뭔지알려</t>
-  </si>
-  <si>
     <t>사주가 너무 충격적이에요</t>
   </si>
   <si>
@@ -5392,9 +5293,6 @@
     <t>갑작스러운 알러지 때문에 긁으면 간지</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출에서 하는 명상의시간이라는... </t>
-  </si>
-  <si>
     <t>급체후 기절을 했습니다</t>
   </si>
   <si>
@@ -5479,9 +5377,6 @@
     <t>선단공포증 때문에 기절한 것 같은데요</t>
   </si>
   <si>
-    <t xml:space="preserve">당혹스러운 금요일을 영어로 어떻게... </t>
-  </si>
-  <si>
     <t>몸에 근육이 자꾸 움찔움찔 움직여요</t>
   </si>
   <si>
@@ -5575,9 +5470,6 @@
     <t xml:space="preserve">다음의 장면중 가장 충격적인 장면은... </t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출 리턴즈 마지막회에 쓰인... </t>
-  </si>
-  <si>
     <t>제동생이기이한경험을했어요</t>
   </si>
   <si>
@@ -5704,9 +5596,6 @@
     <t>그..충격적인 사진보구싶으신 분은</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출 시즌2 삽입곡 질문용... </t>
-  </si>
-  <si>
     <t xml:space="preserve">뜯었는데 반밖에 안들어서 기절할뻔했어... </t>
   </si>
   <si>
@@ -5839,9 +5728,6 @@
     <t xml:space="preserve">먹으면 죽는 약이나 독특하고 기이한... </t>
   </si>
   <si>
-    <t xml:space="preserve">스페인어로 '기이한(또는 희귀한)... </t>
-  </si>
-  <si>
     <t>어제 새벽에 기절..</t>
   </si>
   <si>
@@ -5989,9 +5875,6 @@
     <t>공부할때 깜짝 놀랍니다.</t>
   </si>
   <si>
-    <t>기막힌외출4 어디서 보나요 재밌긴 한가요?</t>
-  </si>
-  <si>
     <t>기절하면서 대변(내공40)</t>
   </si>
   <si>
@@ -6271,9 +6154,6 @@
     <t>제도잖아요. 정부는 기이한 현상인 전세를</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출리턴즈 8회에 사용된 힙합... </t>
-  </si>
-  <si>
     <t>워너원 사진이랑 움찔 좀 주세요.ㅠ</t>
   </si>
   <si>
@@ -6358,9 +6238,6 @@
     <t>갑작스러운 궁금증</t>
   </si>
   <si>
-    <t>기막힌외출예고편에 나오는 음악</t>
-  </si>
-  <si>
     <t>돌렸는데 그뒤로 기억이 안나요 기절해서요</t>
   </si>
   <si>
@@ -6376,9 +6253,6 @@
     <t xml:space="preserve">목디스크로 인한 기절하구 기억이 나질... </t>
   </si>
   <si>
-    <t xml:space="preserve">기절을 발음 그대로 영어로 쓰면 어떻게... </t>
-  </si>
-  <si>
     <t>기지개 펴다 기절</t>
   </si>
   <si>
@@ -6619,9 +6493,6 @@
     <t>크게 절망감을 느끼며 놀란적있습니다.</t>
   </si>
   <si>
-    <t>영어로 "어리둥절.." 과 "이상황은</t>
-  </si>
-  <si>
     <t>물 며칠동안 안마시면 기절하나요?</t>
   </si>
   <si>
@@ -6652,9 +6523,6 @@
     <t>종아리근육이놀란건가</t>
   </si>
   <si>
-    <t>갑작스러운 영어로 ,,, 내공50</t>
-  </si>
-  <si>
     <t>갑작스러운 증상</t>
   </si>
   <si>
@@ -6721,9 +6589,6 @@
     <t>케비에스일일연소큭기막힌유산</t>
   </si>
   <si>
-    <t>들어가면 깜짝 놀래는 링크</t>
-  </si>
-  <si>
     <t>기절하는 동굴..</t>
   </si>
   <si>
@@ -6760,9 +6625,6 @@
     <t>갑자기 움찔</t>
   </si>
   <si>
-    <t>호텔제과제빵과 흠칫</t>
-  </si>
-  <si>
     <t xml:space="preserve">여자친구가 살해 당한 꿈?기절 한 꿈?... </t>
   </si>
   <si>
@@ -6772,9 +6634,6 @@
     <t xml:space="preserve">기절해있을때 누가 물을 먹이면... </t>
   </si>
   <si>
-    <t>기막힌서커스bgm 내공100</t>
-  </si>
-  <si>
     <t>초등학생 기상천외한 오답모음 있자나요...</t>
   </si>
   <si>
@@ -6811,9 +6670,6 @@
     <t>사람이 기절했을때 의사들이 보는 것</t>
   </si>
   <si>
-    <t>"깜짝"을 영어로 적어주세요.. 발음그대로..</t>
-  </si>
-  <si>
     <t>기절놀이를 하다가 아파요</t>
   </si>
   <si>
@@ -7012,9 +6868,6 @@
     <t>기절놀이 뇌 기능 저하</t>
   </si>
   <si>
-    <t>왕과나 즐 기막힌외출 시즌3 짱</t>
-  </si>
-  <si>
     <t>강아지가 자면서 계속 규칙적으로 움찔</t>
   </si>
   <si>
@@ -7126,9 +6979,6 @@
     <t>갑작스러운 몸 안좋아짐</t>
   </si>
   <si>
-    <t>'놀란' 영어로</t>
-  </si>
-  <si>
     <t xml:space="preserve">슈퍼주니어 u 슈퍼주니어 u 충격적인... </t>
   </si>
   <si>
@@ -7612,9 +7462,6 @@
     <t xml:space="preserve">경이로운 용꿈을 꾸었습니다. 해몽 부탁... </t>
   </si>
   <si>
-    <t>기막힌외출 레이싱걸편에서했던거이름좀</t>
-  </si>
-  <si>
     <t>기절에 관하여</t>
   </si>
   <si>
@@ -8134,9 +7981,6 @@
     <t xml:space="preserve">세상에서 가장 충격적인 말을 들었습니다... </t>
   </si>
   <si>
-    <t xml:space="preserve">기이한 일을 보고 고사성어로 뭐라고... </t>
-  </si>
-  <si>
     <t>저는 어깨를 움직일때마다 깜짝 놀랍니다...</t>
   </si>
   <si>
@@ -8206,9 +8050,6 @@
     <t>오디션때.. 당황스러운 질문</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출2-더웃긴밤3에서 해병대편... </t>
-  </si>
-  <si>
     <t xml:space="preserve">동대문노파살인사건 경악 동영상... </t>
   </si>
   <si>
@@ -8434,9 +8275,6 @@
     <t>강정이 기가 막혀에 기막힌 강정은 제</t>
   </si>
   <si>
-    <t>싸이월드 깜짝링크 걸기요.</t>
-  </si>
-  <si>
     <t>'움찔'은 된소리되기가 일어나는 환경</t>
   </si>
   <si>
@@ -8572,9 +8410,6 @@
     <t>교통사고로 놀란것</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출 네버다이7회... </t>
-  </si>
-  <si>
     <t>기이한 꿈을 꾸었습니다</t>
   </si>
   <si>
@@ -8809,9 +8644,6 @@
     <t>당황한 표정을 다른말로</t>
   </si>
   <si>
-    <t>기막힌외출 장동민</t>
-  </si>
-  <si>
     <t xml:space="preserve">헌혈을 하다 기절했는데 제 피는 어떻게... </t>
   </si>
   <si>
@@ -9802,9 +9634,6 @@
     <t>갑작스러운 고열 허리통증 메스꺼움 의</t>
   </si>
   <si>
-    <t>기막힌외출2</t>
-  </si>
-  <si>
     <t xml:space="preserve">깜짝 놀라면 갑자기 스트레스를 받는데... </t>
   </si>
   <si>
@@ -9937,18 +9766,12 @@
     <t xml:space="preserve">백종원의 골목식당 돈까스집에 깜짝손님... </t>
   </si>
   <si>
-    <t xml:space="preserve">Comedy TV 에서 방영중인 기막힌외출... </t>
-  </si>
-  <si>
     <t>작은 소리,,몸짓에도 깜짝 깜짝 놀랩니다...</t>
   </si>
   <si>
     <t>중학생 , 여친한테 깜짝 이벤트..</t>
   </si>
   <si>
-    <t>기절초풍 할것 같다 를 영어로..</t>
-  </si>
-  <si>
     <t>중학생 남친 깜짝생일 이벤트</t>
   </si>
   <si>
@@ -10069,9 +9892,6 @@
     <t>여자울음소리,기절하는 꿈 해몽좀 해주세요</t>
   </si>
   <si>
-    <t>깜짝놀라다 인도네시아어로</t>
-  </si>
-  <si>
     <t>알바 갑작스러운 해고</t>
   </si>
   <si>
@@ -10207,9 +10027,6 @@
     <t xml:space="preserve">충격적이면서도 엽기적인? 그런책을... </t>
   </si>
   <si>
-    <t>기막힌외출시즌3슈퍼주니어</t>
-  </si>
-  <si>
     <t>깜짝 이벤트..?</t>
   </si>
   <si>
@@ -10498,9 +10315,6 @@
     <t>기이한현상인가요?</t>
   </si>
   <si>
-    <t xml:space="preserve">코미디TV 기막힌외출 광고 노래 찾아요... </t>
-  </si>
-  <si>
     <t>기절하는방법 ~</t>
   </si>
   <si>
@@ -10666,9 +10480,6 @@
     <t>아이쿠 내일이 시험이네 중3수학</t>
   </si>
   <si>
-    <t>기막힌외출 명상의시간 동영상좀 ㅜㅜ</t>
-  </si>
-  <si>
     <t>경악토스가 뭔가요?</t>
   </si>
   <si>
@@ -10729,9 +10540,6 @@
     <t>신생아 깜짝놀라는 증상</t>
   </si>
   <si>
-    <t>기막힌외출3 슈퍼주니어....</t>
-  </si>
-  <si>
     <t>갑작스러운 여드름이 나요.</t>
   </si>
   <si>
@@ -10831,9 +10639,6 @@
     <t>중3 화장실에서 기절할뻔했어요</t>
   </si>
   <si>
-    <t>기막힌외출3 이특오빠</t>
-  </si>
-  <si>
     <t>엄마 깜짝 선물</t>
   </si>
   <si>
@@ -11008,9 +10813,6 @@
     <t>기이한 꿈.. 꿈해몽좀 부탁드려요</t>
   </si>
   <si>
-    <t>놀란을영어로머나요?</t>
-  </si>
-  <si>
     <t>갑작스러운 체중 저하</t>
   </si>
   <si>
@@ -11086,9 +10888,6 @@
     <t xml:space="preserve">오피스텔 관리비 명세서를 보고 기겁을... </t>
   </si>
   <si>
-    <t>기막힌외출,댄스정복기에서나온춤</t>
-  </si>
-  <si>
     <t xml:space="preserve">당하며 깜짝 놀랐습니다.(강동 암사동... </t>
   </si>
   <si>
@@ -11149,9 +10948,6 @@
     <t xml:space="preserve">전 진짜 완전 경악먹은게 갓30살아가씨가... </t>
   </si>
   <si>
-    <t>기막힌외출 채널 몇번이에요?</t>
-  </si>
-  <si>
     <t>고혈압 기절하는 방법</t>
   </si>
   <si>
@@ -11287,9 +11083,6 @@
     <t>설리누나의 깜짝 논란</t>
   </si>
   <si>
-    <t xml:space="preserve">ㅠㅠ'깜짝 놀랬는지'를 영어로... </t>
-  </si>
-  <si>
     <t xml:space="preserve">개인적인 생각으로 샌디 코팩스가 놀란... </t>
   </si>
   <si>
@@ -11485,9 +11278,6 @@
     <t>깜짝놀라면심장이빨리크게뛰는이유는?</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출 네버다이 9회에 나온... </t>
-  </si>
-  <si>
     <t>기절 놀이에 대한 정확한 정보 답변 부탁</t>
   </si>
   <si>
@@ -11575,9 +11365,6 @@
     <t xml:space="preserve">이수화학 갑작스러운 상한가 이후... </t>
   </si>
   <si>
-    <t>더웃긴밤3-기막힌외출에 대해서...</t>
-  </si>
-  <si>
     <t>방귀를 참으면 기절을 한다?</t>
   </si>
   <si>
@@ -11737,9 +11524,6 @@
     <t>충격적인그림</t>
   </si>
   <si>
-    <t>기막힌외출에서</t>
-  </si>
-  <si>
     <t>외부 충격으로 인한 기절 후 단기 기억상실?</t>
   </si>
   <si>
@@ -11830,9 +11614,6 @@
     <t>갑작스러운 페업통보</t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출시즌6 해운대에서나온노래인... </t>
-  </si>
-  <si>
     <t>5학년여친한친구깜짝이벤트 내공있음</t>
   </si>
   <si>
@@ -11878,9 +11659,6 @@
     <t xml:space="preserve">공부를 안해요 충격적인말들..그런... </t>
   </si>
   <si>
-    <t>기막힌외출3 다시보기</t>
-  </si>
-  <si>
     <t>깜짝선물 요즘 지쳐하는 남지친구를 위</t>
   </si>
   <si>
@@ -12181,9 +11959,6 @@
     <t>해먹을 수 있는 기막힌 방법을 찾습니다.</t>
   </si>
   <si>
-    <t xml:space="preserve">영어 질문 눈깜짝할사이를 영어단어로... </t>
-  </si>
-  <si>
     <t>강아지가 등을 쓰다듬으면 움찔거려요.</t>
   </si>
   <si>
@@ -12391,9 +12166,6 @@
     <t xml:space="preserve">기상천외한 강아지 이름들.. 최고를... </t>
   </si>
   <si>
-    <t xml:space="preserve">기막힌외출4 2화 9분15초부터나오는... </t>
-  </si>
-  <si>
     <t>잠잘 때 기절할 것 같은 느낌</t>
   </si>
   <si>
@@ -12433,9 +12205,6 @@
     <t>깜짝놀란 고양이짤</t>
   </si>
   <si>
-    <t xml:space="preserve">조금 놀란것뿐이야 아무 감정없어 영어로... </t>
-  </si>
-  <si>
     <t>기절하면서 자면 기면증인가요?</t>
   </si>
   <si>
@@ -12601,9 +12370,6 @@
     <t>가방-0 - 아이쿠 ㅜㅜ</t>
   </si>
   <si>
-    <t>중국어로 깜짝놀랏을때</t>
-  </si>
-  <si>
     <t>저 너무 깜짝놀랐어요..</t>
   </si>
   <si>
@@ -12724,9 +12490,6 @@
     <t xml:space="preserve">우주에서 일어날 수 있는 기이한 현상... </t>
   </si>
   <si>
-    <t xml:space="preserve">슈퍼주니어 사진[슈키라,인탐,기막힌... </t>
-  </si>
-  <si>
     <t>발흠기호표에서 이 기이한 문자들이 뭐죠.?</t>
   </si>
   <si>
@@ -12763,9 +12526,6 @@
     <t>중학교 학생 생기부에 크게 흠칫 갈</t>
   </si>
   <si>
-    <t>기막힌외출 3</t>
-  </si>
-  <si>
     <t>기이한 현상 내공500</t>
   </si>
   <si>
@@ -13292,9 +13052,6 @@
   </si>
   <si>
     <t xml:space="preserve">싸우지않고해결하는 기막힌방법좀알켜주... </t>
-  </si>
-  <si>
-    <t>깜짝 놀라셨죠?는 일본어로 뭐라고 하나요?</t>
   </si>
   <si>
     <t>잠에서 깬 후 놀란것 처럼 심장박동수 증가</t>
@@ -13770,10 +13527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4467"/>
+  <dimension ref="A1:B4386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3403" workbookViewId="0">
-      <selection activeCell="A3419" sqref="A3419"/>
+    <sheetView tabSelected="1" topLeftCell="A4154" workbookViewId="0">
+      <selection activeCell="B4164" sqref="B4164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -48869,654 +48626,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4387" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4387" t="s">
-        <v>4387</v>
-      </c>
-      <c r="B4387" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4388" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4388" t="s">
-        <v>4388</v>
-      </c>
-      <c r="B4388" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4389" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4389" t="s">
-        <v>4389</v>
-      </c>
-      <c r="B4389" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4390" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4390" t="s">
-        <v>4390</v>
-      </c>
-      <c r="B4390" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4391" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4391" t="s">
-        <v>4391</v>
-      </c>
-      <c r="B4391" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4392" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4392" t="s">
-        <v>4392</v>
-      </c>
-      <c r="B4392" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4393" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4393" t="s">
-        <v>4393</v>
-      </c>
-      <c r="B4393" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4394" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4394" t="s">
-        <v>4394</v>
-      </c>
-      <c r="B4394" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4395" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4395" t="s">
-        <v>4395</v>
-      </c>
-      <c r="B4395" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4396" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4396" t="s">
-        <v>4396</v>
-      </c>
-      <c r="B4396" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4397" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4397" t="s">
-        <v>4397</v>
-      </c>
-      <c r="B4397" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4398" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4398" t="s">
-        <v>4398</v>
-      </c>
-      <c r="B4398" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4399" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4399" t="s">
-        <v>4399</v>
-      </c>
-      <c r="B4399" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4400" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4400" t="s">
-        <v>4400</v>
-      </c>
-      <c r="B4400" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4401" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4401" t="s">
-        <v>4401</v>
-      </c>
-      <c r="B4401" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4402" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4402" t="s">
-        <v>4402</v>
-      </c>
-      <c r="B4402" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4403" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4403" t="s">
-        <v>4403</v>
-      </c>
-      <c r="B4403" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4404" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4404" t="s">
-        <v>4404</v>
-      </c>
-      <c r="B4404" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4405" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4405" t="s">
-        <v>4405</v>
-      </c>
-      <c r="B4405" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4406" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4406" t="s">
-        <v>4406</v>
-      </c>
-      <c r="B4406" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4407" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4407" t="s">
-        <v>4407</v>
-      </c>
-      <c r="B4407" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4408" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4408" t="s">
-        <v>4408</v>
-      </c>
-      <c r="B4408" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4409" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4409" t="s">
-        <v>4409</v>
-      </c>
-      <c r="B4409" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4410" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4410" t="s">
-        <v>4410</v>
-      </c>
-      <c r="B4410" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4411" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4411" t="s">
-        <v>4411</v>
-      </c>
-      <c r="B4411" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4412" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4412" t="s">
-        <v>4412</v>
-      </c>
-      <c r="B4412" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4413" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4413" t="s">
-        <v>4413</v>
-      </c>
-      <c r="B4413" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4414" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4414" t="s">
-        <v>4414</v>
-      </c>
-      <c r="B4414" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4415" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4415" t="s">
-        <v>4415</v>
-      </c>
-      <c r="B4415" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4416" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4416" t="s">
-        <v>4416</v>
-      </c>
-      <c r="B4416" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4417" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4417" t="s">
-        <v>4417</v>
-      </c>
-      <c r="B4417" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4418" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4418" t="s">
-        <v>4418</v>
-      </c>
-      <c r="B4418" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4419" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4419" t="s">
-        <v>4419</v>
-      </c>
-      <c r="B4419" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4420" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4420" t="s">
-        <v>4420</v>
-      </c>
-      <c r="B4420" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4421" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4421" t="s">
-        <v>4421</v>
-      </c>
-      <c r="B4421" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4422" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4422" t="s">
-        <v>4422</v>
-      </c>
-      <c r="B4422" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4423" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4423" t="s">
-        <v>4423</v>
-      </c>
-      <c r="B4423" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4424" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4424" t="s">
-        <v>4424</v>
-      </c>
-      <c r="B4424" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4425" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4425" t="s">
-        <v>4425</v>
-      </c>
-      <c r="B4425" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4426" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4426" t="s">
-        <v>4426</v>
-      </c>
-      <c r="B4426" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4427" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4427" t="s">
-        <v>4427</v>
-      </c>
-      <c r="B4427" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4428" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4428" t="s">
-        <v>4428</v>
-      </c>
-      <c r="B4428" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4429" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4429" t="s">
-        <v>4429</v>
-      </c>
-      <c r="B4429" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4430" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4430" t="s">
-        <v>4430</v>
-      </c>
-      <c r="B4430" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4431" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4431" t="s">
-        <v>4431</v>
-      </c>
-      <c r="B4431" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4432" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4432" t="s">
-        <v>4432</v>
-      </c>
-      <c r="B4432" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4433" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4433" t="s">
-        <v>4433</v>
-      </c>
-      <c r="B4433" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4434" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4434" t="s">
-        <v>4434</v>
-      </c>
-      <c r="B4434" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4435" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4435" t="s">
-        <v>4435</v>
-      </c>
-      <c r="B4435" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4436" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4436" t="s">
-        <v>4436</v>
-      </c>
-      <c r="B4436" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4437" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4437" t="s">
-        <v>4437</v>
-      </c>
-      <c r="B4437" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4438" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4438" t="s">
-        <v>4438</v>
-      </c>
-      <c r="B4438" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4439" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4439" t="s">
-        <v>4439</v>
-      </c>
-      <c r="B4439" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4440" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4440" t="s">
-        <v>4440</v>
-      </c>
-      <c r="B4440" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4441" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4441" t="s">
-        <v>4441</v>
-      </c>
-      <c r="B4441" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4442" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4442" t="s">
-        <v>4442</v>
-      </c>
-      <c r="B4442" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4443" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4443" t="s">
-        <v>4443</v>
-      </c>
-      <c r="B4443" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4444" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4444" t="s">
-        <v>4444</v>
-      </c>
-      <c r="B4444" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4445" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4445" t="s">
-        <v>4445</v>
-      </c>
-      <c r="B4445" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4446" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4446" t="s">
-        <v>4446</v>
-      </c>
-      <c r="B4446" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4447" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4447" t="s">
-        <v>4447</v>
-      </c>
-      <c r="B4447" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4448" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4448" t="s">
-        <v>4448</v>
-      </c>
-      <c r="B4448" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4449" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4449" t="s">
-        <v>4449</v>
-      </c>
-      <c r="B4449" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4450" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4450" t="s">
-        <v>4450</v>
-      </c>
-      <c r="B4450" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4451" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4451" t="s">
-        <v>4451</v>
-      </c>
-      <c r="B4451" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4452" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4452" t="s">
-        <v>4452</v>
-      </c>
-      <c r="B4452" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4453" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4453" t="s">
-        <v>4453</v>
-      </c>
-      <c r="B4453" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4454" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4454" t="s">
-        <v>4454</v>
-      </c>
-      <c r="B4454" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4455" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4455" t="s">
-        <v>4455</v>
-      </c>
-      <c r="B4455" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4456" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4456" t="s">
-        <v>4456</v>
-      </c>
-      <c r="B4456" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4457" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4457" t="s">
-        <v>4457</v>
-      </c>
-      <c r="B4457" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4458" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4458" t="s">
-        <v>4458</v>
-      </c>
-      <c r="B4458" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4459" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4459" t="s">
-        <v>4459</v>
-      </c>
-      <c r="B4459" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4460" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4460" t="s">
-        <v>4460</v>
-      </c>
-      <c r="B4460" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4461" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4461" t="s">
-        <v>4461</v>
-      </c>
-      <c r="B4461" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4462" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4462" t="s">
-        <v>4462</v>
-      </c>
-      <c r="B4462" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4463" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4463" t="s">
-        <v>4463</v>
-      </c>
-      <c r="B4463" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4464" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4464" t="s">
-        <v>4464</v>
-      </c>
-      <c r="B4464" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4465" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4465" t="s">
-        <v>4465</v>
-      </c>
-      <c r="B4465" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4466" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4466" t="s">
-        <v>4466</v>
-      </c>
-      <c r="B4466" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4467" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4467" t="s">
-        <v>4467</v>
-      </c>
-      <c r="B4467" t="s">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>